<commit_message>
auto commit 2024-03-19 15:42:41
</commit_message>
<xml_diff>
--- a/pyfutures/universe.xlsx
+++ b/pyfutures/universe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/g1/BU/projects/pytower_develop/pyfutures/pyfutures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D104A5-19E2-3A45-B986-231FE013920C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5B399B-9694-DC48-9586-F3ACCE7E5508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="57100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="universe" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3909" uniqueCount="1127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3911" uniqueCount="1131">
   <si>
     <t>uname</t>
   </si>
@@ -3401,6 +3401,18 @@
   </si>
   <si>
     <t>TODO: implement x day of month for calc roll offset one day roll window, roll day is 3rd Tuesday of the month. Cahgned roll offset from -1 to -3 to pass roll</t>
+  </si>
+  <si>
+    <t>1997N</t>
+  </si>
+  <si>
+    <t>start from U to Z, data is valid from U</t>
+  </si>
+  <si>
+    <t>start from M to N, data is valid from N</t>
+  </si>
+  <si>
+    <t>carry offset: changed start month</t>
   </si>
 </sst>
 </file>
@@ -4272,8 +4284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="AC28" sqref="AC28"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1:AE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4515,7 +4527,7 @@
         <v>-60</v>
       </c>
       <c r="AD2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE2">
         <v>-1</v>
@@ -4635,7 +4647,7 @@
         <v>-60</v>
       </c>
       <c r="AD3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AE3">
         <v>-1</v>
@@ -4749,7 +4761,7 @@
         <v>-60</v>
       </c>
       <c r="AD4">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AE4">
         <v>-1</v>
@@ -4860,7 +4872,7 @@
         <v>-35</v>
       </c>
       <c r="AD5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AE5">
         <v>-1</v>
@@ -4976,7 +4988,7 @@
         <v>-90</v>
       </c>
       <c r="AD6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE6">
         <v>-1</v>
@@ -5083,7 +5095,7 @@
         <v>104</v>
       </c>
       <c r="V7" t="s">
-        <v>105</v>
+        <v>1127</v>
       </c>
       <c r="X7" t="b">
         <v>1</v>
@@ -5104,7 +5116,7 @@
         <v>-60</v>
       </c>
       <c r="AD7">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AE7">
         <v>-1</v>
@@ -5144,6 +5156,9 @@
       </c>
       <c r="AS7" s="1">
         <v>0.80555555555555547</v>
+      </c>
+      <c r="AT7" t="s">
+        <v>1129</v>
       </c>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.2">
@@ -5229,7 +5244,7 @@
         <v>-45</v>
       </c>
       <c r="AD8">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AE8">
         <v>1</v>
@@ -5354,7 +5369,7 @@
         <v>-30</v>
       </c>
       <c r="AD9">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AE9">
         <v>1</v>
@@ -5458,7 +5473,7 @@
         <v>122</v>
       </c>
       <c r="V10" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="X10" t="b">
         <v>1</v>
@@ -5479,7 +5494,7 @@
         <v>-60</v>
       </c>
       <c r="AD10">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE10">
         <v>-1</v>
@@ -5519,6 +5534,9 @@
       </c>
       <c r="AS10" s="1">
         <v>0.80555555555555547</v>
+      </c>
+      <c r="AT10" t="s">
+        <v>1128</v>
       </c>
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.2">
@@ -5604,7 +5622,7 @@
         <v>-90</v>
       </c>
       <c r="AD11">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE11">
         <v>-1</v>
@@ -5732,7 +5750,7 @@
         <v>-90</v>
       </c>
       <c r="AD12">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE12">
         <v>-1</v>
@@ -5860,7 +5878,7 @@
         <v>-90</v>
       </c>
       <c r="AD13">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE13">
         <v>-1</v>
@@ -5982,7 +6000,7 @@
         <v>-90</v>
       </c>
       <c r="AD14">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE14">
         <v>-1</v>
@@ -6101,7 +6119,7 @@
         <v>-60</v>
       </c>
       <c r="AD15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AE15">
         <v>-1</v>
@@ -6229,7 +6247,7 @@
         <v>-60</v>
       </c>
       <c r="AD16">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="AE16">
         <v>-1</v>
@@ -6399,7 +6417,7 @@
         <v>0.79513888888888884</v>
       </c>
       <c r="AT17" t="s">
-        <v>58</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="18" spans="1:46" x14ac:dyDescent="0.2">
@@ -6485,7 +6503,7 @@
         <v>-60</v>
       </c>
       <c r="AD18">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AE18">
         <v>-1</v>
@@ -6616,7 +6634,7 @@
         <v>-60</v>
       </c>
       <c r="AD19">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AE19">
         <v>-1</v>
@@ -6736,7 +6754,7 @@
         <v>-50</v>
       </c>
       <c r="AD20">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AE20">
         <v>-1</v>
@@ -6859,7 +6877,7 @@
         <v>-50</v>
       </c>
       <c r="AD21">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AE21">
         <v>-1</v>
@@ -6979,7 +6997,7 @@
         <v>-60</v>
       </c>
       <c r="AD22">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="AE22">
         <v>-1</v>
@@ -7107,7 +7125,7 @@
         <v>-50</v>
       </c>
       <c r="AD23">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AE23">
         <v>-1</v>
@@ -7235,7 +7253,7 @@
         <v>-60</v>
       </c>
       <c r="AD24">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AE24">
         <v>-1</v>
@@ -7363,7 +7381,7 @@
         <v>-50</v>
       </c>
       <c r="AD25">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AE25">
         <v>-1</v>
@@ -7491,7 +7509,7 @@
         <v>-40</v>
       </c>
       <c r="AD26">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AE26">
         <v>1</v>
@@ -7616,7 +7634,7 @@
         <v>-60</v>
       </c>
       <c r="AD27">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="AE27">
         <v>-1</v>
@@ -7736,7 +7754,7 @@
         <v>-3</v>
       </c>
       <c r="AD28">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE28">
         <v>1</v>
@@ -7856,7 +7874,7 @@
         <v>-20</v>
       </c>
       <c r="AD29">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE29">
         <v>1</v>
@@ -7964,7 +7982,7 @@
         <v>-20</v>
       </c>
       <c r="AD30">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE30">
         <v>1</v>
@@ -8072,7 +8090,7 @@
         <v>-20</v>
       </c>
       <c r="AD31">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE31">
         <v>1</v>
@@ -8180,7 +8198,7 @@
         <v>-5</v>
       </c>
       <c r="AD32">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE32">
         <v>1</v>
@@ -8288,7 +8306,7 @@
         <v>-5</v>
       </c>
       <c r="AD33">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AE33">
         <v>1</v>
@@ -8405,7 +8423,7 @@
         <v>-5</v>
       </c>
       <c r="AD34">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AE34">
         <v>1</v>
@@ -8522,7 +8540,7 @@
         <v>-5</v>
       </c>
       <c r="AD35">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AE35">
         <v>1</v>
@@ -8639,7 +8657,7 @@
         <v>-5</v>
       </c>
       <c r="AD36">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AE36">
         <v>1</v>
@@ -8756,7 +8774,7 @@
         <v>-36</v>
       </c>
       <c r="AD37">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AE37">
         <v>1</v>
@@ -8876,7 +8894,7 @@
         <v>-5</v>
       </c>
       <c r="AD38">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AE38">
         <v>1</v>
@@ -8993,7 +9011,7 @@
         <v>-5</v>
       </c>
       <c r="AD39">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AE39">
         <v>1</v>
@@ -9118,7 +9136,7 @@
         <v>-25</v>
       </c>
       <c r="AD40">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AE40">
         <v>1</v>
@@ -9239,7 +9257,7 @@
         <v>-20</v>
       </c>
       <c r="AD41">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE41">
         <v>1</v>
@@ -9364,7 +9382,7 @@
         <v>-25</v>
       </c>
       <c r="AD42">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AE42">
         <v>1</v>
@@ -9480,7 +9498,7 @@
         <v>-25</v>
       </c>
       <c r="AD43">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AE43">
         <v>1</v>
@@ -9596,7 +9614,7 @@
         <v>-25</v>
       </c>
       <c r="AD44">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AE44">
         <v>1</v>
@@ -9721,7 +9739,7 @@
         <v>-25</v>
       </c>
       <c r="AD45">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AE45">
         <v>1</v>
@@ -9846,7 +9864,7 @@
         <v>-25</v>
       </c>
       <c r="AD46">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AE46">
         <v>1</v>
@@ -9963,7 +9981,7 @@
         <v>-45</v>
       </c>
       <c r="AD47">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AE47">
         <v>-1</v>
@@ -10074,7 +10092,7 @@
         <v>-270</v>
       </c>
       <c r="AD48">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE48">
         <v>-1</v>
@@ -10194,7 +10212,7 @@
         <v>-60</v>
       </c>
       <c r="AD49">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="AE49">
         <v>-1</v>
@@ -10305,7 +10323,7 @@
         <v>-60</v>
       </c>
       <c r="AD50">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="AE50">
         <v>-1</v>
@@ -10433,7 +10451,7 @@
         <v>-35</v>
       </c>
       <c r="AD51">
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="AE51">
         <v>-1</v>
@@ -10561,7 +10579,7 @@
         <v>-35</v>
       </c>
       <c r="AD52">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="AE52">
         <v>-1</v>
@@ -10689,7 +10707,7 @@
         <v>-35</v>
       </c>
       <c r="AD53">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="AE53">
         <v>-1</v>
@@ -10817,7 +10835,7 @@
         <v>-40</v>
       </c>
       <c r="AD54">
-        <v>-32</v>
+        <v>-31</v>
       </c>
       <c r="AE54">
         <v>-1</v>
@@ -10928,7 +10946,7 @@
         <v>-15</v>
       </c>
       <c r="AD55">
-        <v>-32</v>
+        <v>-31</v>
       </c>
       <c r="AE55">
         <v>-1</v>
@@ -11039,7 +11057,7 @@
         <v>-15</v>
       </c>
       <c r="AD56">
-        <v>-32</v>
+        <v>-31</v>
       </c>
       <c r="AE56">
         <v>-1</v>
@@ -11150,7 +11168,7 @@
         <v>-60</v>
       </c>
       <c r="AD57">
-        <v>-32</v>
+        <v>-31</v>
       </c>
       <c r="AE57">
         <v>-1</v>
@@ -11269,7 +11287,7 @@
         <v>-40</v>
       </c>
       <c r="AD58">
-        <v>-11</v>
+        <v>-10</v>
       </c>
       <c r="AE58">
         <v>-1</v>
@@ -11394,7 +11412,7 @@
         <v>-60</v>
       </c>
       <c r="AD59">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE59">
         <v>-1</v>
@@ -11522,7 +11540,7 @@
         <v>-40</v>
       </c>
       <c r="AD60">
-        <v>-11</v>
+        <v>-10</v>
       </c>
       <c r="AE60">
         <v>-1</v>
@@ -11650,7 +11668,7 @@
         <v>-40</v>
       </c>
       <c r="AD61">
-        <v>-11</v>
+        <v>-10</v>
       </c>
       <c r="AE61">
         <v>-1</v>
@@ -11778,7 +11796,7 @@
         <v>-60</v>
       </c>
       <c r="AD62">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE62">
         <v>-1</v>
@@ -11898,7 +11916,7 @@
         <v>-5</v>
       </c>
       <c r="AD63">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AE63">
         <v>1</v>
@@ -12012,7 +12030,7 @@
         <v>-10</v>
       </c>
       <c r="AD64">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AE64">
         <v>1</v>
@@ -12126,7 +12144,7 @@
         <v>-10</v>
       </c>
       <c r="AD65">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE65">
         <v>1</v>
@@ -12246,7 +12264,7 @@
         <v>-10</v>
       </c>
       <c r="AD66">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE66">
         <v>1</v>
@@ -12366,7 +12384,7 @@
         <v>-1</v>
       </c>
       <c r="AD67">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AE67">
         <v>1</v>
@@ -12486,7 +12504,7 @@
         <v>-1</v>
       </c>
       <c r="AD68">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AE68">
         <v>1</v>
@@ -12606,7 +12624,7 @@
         <v>-5</v>
       </c>
       <c r="AD69">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AE69">
         <v>1</v>
@@ -12723,7 +12741,7 @@
         <v>-5</v>
       </c>
       <c r="AD70">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AE70">
         <v>1</v>
@@ -12843,7 +12861,7 @@
         <v>-10</v>
       </c>
       <c r="AD71">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AE71">
         <v>1</v>
@@ -12968,7 +12986,7 @@
         <v>-6</v>
       </c>
       <c r="AD72">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AE72">
         <v>1</v>
@@ -13096,7 +13114,7 @@
         <v>-5</v>
       </c>
       <c r="AD73">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE73">
         <v>1</v>
@@ -13213,7 +13231,7 @@
         <v>-5</v>
       </c>
       <c r="AD74">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AE74">
         <v>1</v>
@@ -13333,7 +13351,7 @@
         <v>-5</v>
       </c>
       <c r="AD75">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AE75">
         <v>1</v>
@@ -13453,7 +13471,7 @@
         <v>-5</v>
       </c>
       <c r="AD76">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AE76">
         <v>1</v>
@@ -13573,7 +13591,7 @@
         <v>-5</v>
       </c>
       <c r="AD77">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AE77">
         <v>1</v>
@@ -13690,7 +13708,7 @@
         <v>-5</v>
       </c>
       <c r="AD78">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AE78">
         <v>1</v>
@@ -13813,7 +13831,7 @@
         <v>-8</v>
       </c>
       <c r="AD79">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AE79">
         <v>1</v>
@@ -13936,7 +13954,7 @@
         <v>-8</v>
       </c>
       <c r="AD80">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AE80">
         <v>1</v>
@@ -14056,7 +14074,7 @@
         <v>-5</v>
       </c>
       <c r="AD81">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AE81">
         <v>1</v>
@@ -14176,7 +14194,7 @@
         <v>-5</v>
       </c>
       <c r="AD82">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AE82">
         <v>1</v>
@@ -14296,7 +14314,7 @@
         <v>-5</v>
       </c>
       <c r="AD83">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AE83">
         <v>1</v>
@@ -14416,7 +14434,7 @@
         <v>-5</v>
       </c>
       <c r="AD84">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE84">
         <v>1</v>
@@ -14533,7 +14551,7 @@
         <v>-5</v>
       </c>
       <c r="AD85">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE85">
         <v>1</v>
@@ -14650,7 +14668,7 @@
         <v>-5</v>
       </c>
       <c r="AD86">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE86">
         <v>1</v>
@@ -14767,7 +14785,7 @@
         <v>-30</v>
       </c>
       <c r="AD87">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AE87">
         <v>1</v>
@@ -14887,7 +14905,7 @@
         <v>-5</v>
       </c>
       <c r="AD88">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE88">
         <v>1</v>
@@ -15004,7 +15022,7 @@
         <v>-5</v>
       </c>
       <c r="AD89">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AE89">
         <v>1</v>
@@ -15124,7 +15142,7 @@
         <v>-5</v>
       </c>
       <c r="AD90">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AE90">
         <v>1</v>
@@ -15244,7 +15262,7 @@
         <v>-5</v>
       </c>
       <c r="AD91">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AE91">
         <v>1</v>
@@ -15364,7 +15382,7 @@
         <v>-10</v>
       </c>
       <c r="AD92">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE92">
         <v>1</v>
@@ -15484,7 +15502,7 @@
         <v>-5</v>
       </c>
       <c r="AD93">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE93">
         <v>1</v>
@@ -15601,7 +15619,7 @@
         <v>-5</v>
       </c>
       <c r="AD94">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE94">
         <v>1</v>
@@ -15721,7 +15739,7 @@
         <v>-5</v>
       </c>
       <c r="AD95">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE95">
         <v>1</v>
@@ -15844,7 +15862,7 @@
         <v>-10</v>
       </c>
       <c r="AD96">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AE96">
         <v>1</v>
@@ -15964,7 +15982,7 @@
         <v>-5</v>
       </c>
       <c r="AD97">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE97">
         <v>1</v>
@@ -16084,7 +16102,7 @@
         <v>-5</v>
       </c>
       <c r="AD98">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE98">
         <v>1</v>
@@ -16204,7 +16222,7 @@
         <v>-5</v>
       </c>
       <c r="AD99">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE99">
         <v>1</v>
@@ -16324,7 +16342,7 @@
         <v>-5</v>
       </c>
       <c r="AD100">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE100">
         <v>1</v>
@@ -16444,7 +16462,7 @@
         <v>-5</v>
       </c>
       <c r="AD101">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE101">
         <v>1</v>
@@ -16564,7 +16582,7 @@
         <v>-10</v>
       </c>
       <c r="AD102">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AE102">
         <v>1</v>
@@ -16681,7 +16699,7 @@
         <v>-5</v>
       </c>
       <c r="AD103">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE103">
         <v>1</v>
@@ -16801,7 +16819,7 @@
         <v>-5</v>
       </c>
       <c r="AD104">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE104">
         <v>1</v>
@@ -16926,7 +16944,7 @@
         <v>-5</v>
       </c>
       <c r="AD105">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE105">
         <v>1</v>
@@ -17051,7 +17069,7 @@
         <v>-5</v>
       </c>
       <c r="AD106">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE106">
         <v>1</v>
@@ -17176,7 +17194,7 @@
         <v>-5</v>
       </c>
       <c r="AD107">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE107">
         <v>1</v>
@@ -17301,7 +17319,7 @@
         <v>-5</v>
       </c>
       <c r="AD108">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE108">
         <v>1</v>
@@ -17426,7 +17444,7 @@
         <v>-5</v>
       </c>
       <c r="AD109">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE109">
         <v>1</v>
@@ -17547,7 +17565,7 @@
         <v>-5</v>
       </c>
       <c r="AD110">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE110">
         <v>1</v>
@@ -17668,7 +17686,7 @@
         <v>-5</v>
       </c>
       <c r="AD111">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE111">
         <v>1</v>
@@ -17796,7 +17814,7 @@
         <v>-6</v>
       </c>
       <c r="AD112">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AE112">
         <v>1</v>
@@ -17924,7 +17942,7 @@
         <v>-5</v>
       </c>
       <c r="AD113">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE113">
         <v>1</v>
@@ -18043,7 +18061,7 @@
         <v>-7</v>
       </c>
       <c r="AD114">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AE114">
         <v>1</v>
@@ -18168,7 +18186,7 @@
         <v>-5</v>
       </c>
       <c r="AD115">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AE115">
         <v>1</v>
@@ -18293,7 +18311,7 @@
         <v>-5</v>
       </c>
       <c r="AD116">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE116">
         <v>1</v>
@@ -18421,7 +18439,7 @@
         <v>-5</v>
       </c>
       <c r="AD117">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AE117">
         <v>1</v>
@@ -18541,7 +18559,7 @@
         <v>-10</v>
       </c>
       <c r="AD118">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE118">
         <v>1</v>
@@ -18652,7 +18670,7 @@
         <v>-10</v>
       </c>
       <c r="AD119">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE119">
         <v>1</v>
@@ -18763,7 +18781,7 @@
         <v>-10</v>
       </c>
       <c r="AD120">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE120">
         <v>1</v>
@@ -18882,7 +18900,7 @@
         <v>-6</v>
       </c>
       <c r="AD121">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE121">
         <v>1</v>
@@ -19010,7 +19028,7 @@
         <v>-5</v>
       </c>
       <c r="AD122">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AE122">
         <v>1</v>
@@ -19138,7 +19156,7 @@
         <v>-5</v>
       </c>
       <c r="AD123">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AE123">
         <v>1</v>
@@ -19263,7 +19281,7 @@
         <v>-30</v>
       </c>
       <c r="AD124">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AE124">
         <v>1</v>
@@ -19379,7 +19397,7 @@
         <v>-5</v>
       </c>
       <c r="AD125">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AE125">
         <v>1</v>
@@ -19504,7 +19522,7 @@
         <v>-5</v>
       </c>
       <c r="AD126">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AE126">
         <v>1</v>
@@ -19629,7 +19647,7 @@
         <v>-5</v>
       </c>
       <c r="AD127">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AE127">
         <v>1</v>
@@ -19754,7 +19772,7 @@
         <v>-5</v>
       </c>
       <c r="AD128">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AE128">
         <v>1</v>
@@ -19879,7 +19897,7 @@
         <v>-5</v>
       </c>
       <c r="AD129">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE129">
         <v>1</v>
@@ -20007,7 +20025,7 @@
         <v>-5</v>
       </c>
       <c r="AD130">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AE130">
         <v>1</v>
@@ -20132,7 +20150,7 @@
         <v>-10</v>
       </c>
       <c r="AD131">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AE131">
         <v>1</v>
@@ -20249,7 +20267,7 @@
         <v>-60</v>
       </c>
       <c r="AD132">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AE132">
         <v>-1</v>
@@ -20369,7 +20387,7 @@
         <v>-30</v>
       </c>
       <c r="AD133">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AE133">
         <v>1</v>
@@ -20494,7 +20512,7 @@
         <v>-45</v>
       </c>
       <c r="AD134">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE134">
         <v>1</v>
@@ -20619,7 +20637,7 @@
         <v>-30</v>
       </c>
       <c r="AD135">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AE135">
         <v>1</v>
@@ -20744,7 +20762,7 @@
         <v>-90</v>
       </c>
       <c r="AD136">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE136">
         <v>-1</v>
@@ -20863,7 +20881,7 @@
         <v>-30</v>
       </c>
       <c r="AD137">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE137">
         <v>1</v>
@@ -20988,7 +21006,7 @@
         <v>-30</v>
       </c>
       <c r="AD138">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AE138">
         <v>1</v>
@@ -21113,7 +21131,7 @@
         <v>-30</v>
       </c>
       <c r="AD139">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AE139">
         <v>1</v>
@@ -21238,7 +21256,7 @@
         <v>-4</v>
       </c>
       <c r="AD140">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AE140">
         <v>1</v>
@@ -21357,7 +21375,7 @@
         <v>-30</v>
       </c>
       <c r="AD141">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AE141">
         <v>1</v>
@@ -21482,7 +21500,7 @@
         <v>-30</v>
       </c>
       <c r="AD142">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AE142">
         <v>1</v>
@@ -21607,7 +21625,7 @@
         <v>-45</v>
       </c>
       <c r="AD143">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AE143">
         <v>-1</v>
@@ -21735,7 +21753,7 @@
         <v>-45</v>
       </c>
       <c r="AD144">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AE144">
         <v>-1</v>
@@ -21863,7 +21881,7 @@
         <v>-18</v>
       </c>
       <c r="AD145">
-        <v>1843</v>
+        <v>1844</v>
       </c>
       <c r="AE145">
         <v>1</v>
@@ -21980,7 +21998,7 @@
         <v>-700</v>
       </c>
       <c r="AD146">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE146">
         <v>-1</v>
@@ -22091,7 +22109,7 @@
         <v>-700</v>
       </c>
       <c r="AD147">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE147">
         <v>-1</v>
@@ -22202,7 +22220,7 @@
         <v>-1000</v>
       </c>
       <c r="AD148">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AE148">
         <v>-1</v>
@@ -22321,7 +22339,7 @@
         <v>-1000</v>
       </c>
       <c r="AD149">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AE149">
         <v>-1</v>
@@ -22444,7 +22462,7 @@
         <v>-60</v>
       </c>
       <c r="AD150">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AE150">
         <v>-1</v>
@@ -22569,7 +22587,7 @@
         <v>-60</v>
       </c>
       <c r="AD151">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AE151">
         <v>-1</v>
@@ -22694,7 +22712,7 @@
         <v>-60</v>
       </c>
       <c r="AD152">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AE152">
         <v>-1</v>
@@ -22811,7 +22829,7 @@
         <v>-5</v>
       </c>
       <c r="AD153">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE153">
         <v>1</v>

</xml_diff>

<commit_message>
auto commit 2024-03-19 17:26:49
</commit_message>
<xml_diff>
--- a/pyfutures/universe.xlsx
+++ b/pyfutures/universe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/g1/BU/projects/pytower_develop/pyfutures/pyfutures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5B399B-9694-DC48-9586-F3ACCE7E5508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43ADAAD-2E6E-DD40-8DD7-B95EDFF32A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="57100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="universe" sheetId="1" r:id="rId1"/>
@@ -4284,8 +4284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1:AE1048576"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="AC64" sqref="AC64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
auto commit 2024-03-19 17:29:09
</commit_message>
<xml_diff>
--- a/pyfutures/universe.xlsx
+++ b/pyfutures/universe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/g1/BU/projects/pytower_develop/pyfutures/pyfutures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43ADAAD-2E6E-DD40-8DD7-B95EDFF32A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AF1E7D-573F-7147-903B-714BBCCC575C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="57100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3911" uniqueCount="1131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3910" uniqueCount="1131">
   <si>
     <t>uname</t>
   </si>
@@ -4284,8 +4284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="AC64" sqref="AC64"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="F153" sqref="F153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21800,76 +21800,68 @@
     </row>
     <row r="145" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>995</v>
+        <v>1001</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>89</v>
+        <v>315</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>995</v>
+        <v>1000</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>995</v>
+        <v>1002</v>
       </c>
       <c r="H145" t="s">
-        <v>45</v>
+        <v>258</v>
       </c>
       <c r="I145" t="s">
-        <v>997</v>
-      </c>
-      <c r="J145" s="6" t="s">
-        <v>1119</v>
+        <v>1005</v>
+      </c>
+      <c r="J145" s="3" t="s">
+        <v>1116</v>
       </c>
       <c r="K145" s="5">
-        <v>0.85</v>
+        <v>2</v>
       </c>
       <c r="L145" s="5" t="s">
-        <v>45</v>
+        <v>258</v>
       </c>
       <c r="M145" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="N145" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="O145" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="P145" s="5">
-        <v>0.02</v>
-      </c>
-      <c r="Q145" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="N145" s="5"/>
+      <c r="O145" s="5"/>
+      <c r="P145" s="5"/>
+      <c r="Q145" s="5"/>
       <c r="R145" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="S145">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="T145" t="s">
-        <v>996</v>
+        <v>1003</v>
       </c>
       <c r="U145" t="s">
-        <v>996</v>
+        <v>1003</v>
       </c>
       <c r="V145" t="s">
-        <v>996</v>
+        <v>1004</v>
       </c>
       <c r="X145" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y145">
         <v>1</v>
       </c>
       <c r="Z145">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AA145" t="s">
         <v>272</v>
@@ -21878,66 +21870,60 @@
         <v>272</v>
       </c>
       <c r="AC145">
-        <v>-18</v>
+        <v>-700</v>
       </c>
       <c r="AD145">
-        <v>1844</v>
+        <v>16</v>
       </c>
       <c r="AE145">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AF145" t="s">
-        <v>50</v>
+        <v>318</v>
       </c>
       <c r="AG145" t="s">
-        <v>51</v>
+        <v>318</v>
       </c>
       <c r="AH145" t="s">
-        <v>370</v>
+        <v>326</v>
       </c>
       <c r="AI145" s="1">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="AJ145">
-        <v>22</v>
+        <v>0.71875</v>
       </c>
       <c r="AL145" t="s">
         <v>998</v>
       </c>
       <c r="AM145" t="s">
-        <v>277</v>
+        <v>359</v>
       </c>
       <c r="AN145" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="AO145" t="s">
-        <v>999</v>
+        <v>1006</v>
       </c>
       <c r="AQ145">
-        <v>1000</v>
-      </c>
-      <c r="AR145" s="1">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="AS145" s="1">
-        <v>0.91666666666666663</v>
+        <v>2500</v>
+      </c>
+      <c r="AT145" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="146" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
-        <v>1000</v>
+        <v>1007</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>1000</v>
+        <v>1007</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>1001</v>
+        <v>1007</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>315</v>
+        <v>344</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>1000</v>
+        <v>1007</v>
       </c>
       <c r="F146" s="3" t="s">
         <v>1002</v>
@@ -21946,13 +21932,13 @@
         <v>258</v>
       </c>
       <c r="I146" t="s">
-        <v>1005</v>
+        <v>1009</v>
       </c>
       <c r="J146" s="3" t="s">
-        <v>1116</v>
+        <v>1095</v>
       </c>
       <c r="K146" s="5">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="L146" s="5" t="s">
         <v>258</v>
@@ -21965,7 +21951,7 @@
       <c r="P146" s="5"/>
       <c r="Q146" s="5"/>
       <c r="R146" t="s">
-        <v>63</v>
+        <v>193</v>
       </c>
       <c r="S146">
         <v>5.0000000000000001E-3</v>
@@ -22004,16 +21990,16 @@
         <v>-1</v>
       </c>
       <c r="AF146" t="s">
-        <v>318</v>
+        <v>663</v>
       </c>
       <c r="AG146" t="s">
-        <v>318</v>
+        <v>1008</v>
       </c>
       <c r="AH146" t="s">
-        <v>326</v>
+        <v>665</v>
       </c>
       <c r="AI146" s="1">
-        <v>0.71875</v>
+        <v>0.68055555555555547</v>
       </c>
       <c r="AL146" t="s">
         <v>998</v>
@@ -22025,7 +22011,7 @@
         <v>72</v>
       </c>
       <c r="AO146" t="s">
-        <v>1006</v>
+        <v>1010</v>
       </c>
       <c r="AQ146">
         <v>2500</v>
@@ -22036,37 +22022,37 @@
     </row>
     <row r="147" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
-        <v>1007</v>
+        <v>1011</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>1007</v>
+        <v>1011</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>1007</v>
+        <v>1012</v>
       </c>
       <c r="D147" s="3" t="s">
         <v>344</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>1007</v>
+        <v>1011</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>1002</v>
+        <v>1011</v>
       </c>
       <c r="H147" t="s">
-        <v>258</v>
+        <v>147</v>
       </c>
       <c r="I147" t="s">
-        <v>1009</v>
+        <v>1015</v>
       </c>
       <c r="J147" s="3" t="s">
         <v>1095</v>
       </c>
       <c r="K147" s="5">
-        <v>2.5</v>
+        <v>1.7</v>
       </c>
       <c r="L147" s="5" t="s">
-        <v>258</v>
+        <v>147</v>
       </c>
       <c r="M147" s="5" t="b">
         <v>0</v>
@@ -22082,13 +22068,13 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="T147" t="s">
-        <v>1003</v>
+        <v>737</v>
       </c>
       <c r="U147" t="s">
-        <v>1003</v>
+        <v>737</v>
       </c>
       <c r="V147" t="s">
-        <v>1004</v>
+        <v>1013</v>
       </c>
       <c r="X147" t="b">
         <v>1</v>
@@ -22097,7 +22083,7 @@
         <v>1</v>
       </c>
       <c r="Z147">
-        <v>5.0000000000000001E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="AA147" t="s">
         <v>272</v>
@@ -22106,22 +22092,22 @@
         <v>272</v>
       </c>
       <c r="AC147">
-        <v>-700</v>
+        <v>-1000</v>
       </c>
       <c r="AD147">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="AE147">
         <v>-1</v>
       </c>
       <c r="AF147" t="s">
-        <v>663</v>
+        <v>1008</v>
       </c>
       <c r="AG147" t="s">
         <v>1008</v>
       </c>
       <c r="AH147" t="s">
-        <v>665</v>
+        <v>1014</v>
       </c>
       <c r="AI147" s="1">
         <v>0.68055555555555547</v>
@@ -22136,7 +22122,7 @@
         <v>72</v>
       </c>
       <c r="AO147" t="s">
-        <v>1010</v>
+        <v>1016</v>
       </c>
       <c r="AQ147">
         <v>2500</v>
@@ -22147,47 +22133,55 @@
     </row>
     <row r="148" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
-        <v>1011</v>
+        <v>1017</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>1011</v>
+        <v>1017</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>1012</v>
+        <v>1018</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>344</v>
+        <v>43</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>1011</v>
+        <v>1017</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>1011</v>
+        <v>1017</v>
       </c>
       <c r="H148" t="s">
-        <v>147</v>
+        <v>45</v>
       </c>
       <c r="I148" t="s">
-        <v>1015</v>
-      </c>
-      <c r="J148" s="3" t="s">
-        <v>1095</v>
+        <v>1019</v>
+      </c>
+      <c r="J148" s="6" t="s">
+        <v>1119</v>
       </c>
       <c r="K148" s="5">
-        <v>1.7</v>
+        <v>0.85</v>
       </c>
       <c r="L148" s="5" t="s">
-        <v>147</v>
+        <v>45</v>
       </c>
       <c r="M148" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="N148" s="5"/>
-      <c r="O148" s="5"/>
-      <c r="P148" s="5"/>
-      <c r="Q148" s="5"/>
+      <c r="N148" s="5">
+        <v>1.25</v>
+      </c>
+      <c r="O148" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P148" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="Q148" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="R148" t="s">
-        <v>193</v>
+        <v>46</v>
       </c>
       <c r="S148">
         <v>5.0000000000000001E-3</v>
@@ -22220,22 +22214,25 @@
         <v>-1000</v>
       </c>
       <c r="AD148">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="AE148">
         <v>-1</v>
       </c>
       <c r="AF148" t="s">
-        <v>1008</v>
+        <v>50</v>
       </c>
       <c r="AG148" t="s">
-        <v>1008</v>
+        <v>377</v>
       </c>
       <c r="AH148" t="s">
-        <v>1014</v>
+        <v>370</v>
       </c>
       <c r="AI148" s="1">
-        <v>0.68055555555555547</v>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="AJ148">
+        <v>22</v>
       </c>
       <c r="AL148" t="s">
         <v>998</v>
@@ -22244,81 +22241,82 @@
         <v>359</v>
       </c>
       <c r="AN148" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="AO148" t="s">
-        <v>1016</v>
+        <v>1020</v>
       </c>
       <c r="AQ148">
         <v>2500</v>
       </c>
+      <c r="AR148" s="1">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="AS148" s="1">
+        <v>0.91666666666666663</v>
+      </c>
       <c r="AT148" t="s">
-        <v>58</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="149" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
-        <v>1017</v>
+        <v>1022</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>1017</v>
+        <v>1022</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>1018</v>
+        <v>1023</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>43</v>
+        <v>315</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>1017</v>
+        <v>1022</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>1017</v>
+        <v>1022</v>
       </c>
       <c r="H149" t="s">
-        <v>45</v>
+        <v>258</v>
       </c>
       <c r="I149" t="s">
-        <v>1019</v>
-      </c>
-      <c r="J149" s="6" t="s">
-        <v>1119</v>
+        <v>1028</v>
+      </c>
+      <c r="J149" s="3" t="s">
+        <v>1085</v>
       </c>
       <c r="K149" s="5">
-        <v>0.85</v>
+        <v>2</v>
       </c>
       <c r="L149" s="5" t="s">
-        <v>45</v>
+        <v>258</v>
       </c>
       <c r="M149" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="N149" s="5">
-        <v>1.25</v>
-      </c>
-      <c r="O149" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="P149" s="5">
-        <v>0.02</v>
-      </c>
-      <c r="Q149" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="N149" s="5"/>
+      <c r="O149" s="5"/>
+      <c r="P149" s="5"/>
+      <c r="Q149" s="5"/>
       <c r="R149" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="S149">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="T149" t="s">
-        <v>737</v>
+        <v>1024</v>
       </c>
       <c r="U149" t="s">
-        <v>737</v>
+        <v>1024</v>
       </c>
       <c r="V149" t="s">
-        <v>1013</v>
+        <v>389</v>
+      </c>
+      <c r="W149" t="s">
+        <v>1025</v>
       </c>
       <c r="X149" t="b">
         <v>1</v>
@@ -22327,121 +22325,123 @@
         <v>1</v>
       </c>
       <c r="Z149">
-        <v>2.5000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="AA149" t="s">
-        <v>272</v>
+        <v>49</v>
       </c>
       <c r="AB149" t="s">
-        <v>272</v>
+        <v>49</v>
       </c>
       <c r="AC149">
-        <v>-1000</v>
+        <v>-60</v>
       </c>
       <c r="AD149">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AE149">
         <v>-1</v>
       </c>
       <c r="AF149" t="s">
-        <v>50</v>
+        <v>1026</v>
       </c>
       <c r="AG149" t="s">
-        <v>377</v>
+        <v>207</v>
       </c>
       <c r="AH149" t="s">
-        <v>370</v>
+        <v>1027</v>
       </c>
       <c r="AI149" s="1">
-        <v>0.58333333333333337</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="AJ149">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AL149" t="s">
-        <v>998</v>
-      </c>
-      <c r="AM149" t="s">
-        <v>359</v>
+        <v>1029</v>
       </c>
       <c r="AN149" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="AO149" t="s">
-        <v>1020</v>
+        <v>1030</v>
       </c>
       <c r="AQ149">
-        <v>2500</v>
+        <v>100</v>
       </c>
       <c r="AR149" s="1">
-        <v>0.29166666666666669</v>
+        <v>5.2083333333333336E-2</v>
       </c>
       <c r="AS149" s="1">
-        <v>0.91666666666666663</v>
+        <v>0.875</v>
       </c>
       <c r="AT149" t="s">
-        <v>1021</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="150" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
-        <v>1022</v>
+        <v>1032</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>1022</v>
+        <v>1032</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>1023</v>
+        <v>1033</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>315</v>
+        <v>1034</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>1022</v>
+        <v>1032</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>1022</v>
+        <v>1032</v>
       </c>
       <c r="H150" t="s">
-        <v>258</v>
+        <v>45</v>
       </c>
       <c r="I150" t="s">
-        <v>1028</v>
-      </c>
-      <c r="J150" s="3" t="s">
-        <v>1085</v>
+        <v>1036</v>
+      </c>
+      <c r="J150" s="6" t="s">
+        <v>1119</v>
       </c>
       <c r="K150" s="5">
-        <v>2</v>
+        <v>0.85</v>
       </c>
       <c r="L150" s="5" t="s">
-        <v>258</v>
+        <v>45</v>
       </c>
       <c r="M150" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="N150" s="5"/>
-      <c r="O150" s="5"/>
-      <c r="P150" s="5"/>
-      <c r="Q150" s="5"/>
+      <c r="N150" s="5">
+        <v>1.47</v>
+      </c>
+      <c r="O150" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P150" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="Q150" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="R150" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="S150">
         <v>0.05</v>
       </c>
       <c r="T150" t="s">
-        <v>1024</v>
+        <v>78</v>
       </c>
       <c r="U150" t="s">
-        <v>1024</v>
+        <v>78</v>
       </c>
       <c r="V150" t="s">
-        <v>389</v>
-      </c>
-      <c r="W150" t="s">
-        <v>1025</v>
+        <v>1035</v>
       </c>
       <c r="X150" t="b">
         <v>1</v>
@@ -22468,57 +22468,57 @@
         <v>-1</v>
       </c>
       <c r="AF150" t="s">
-        <v>1026</v>
+        <v>50</v>
       </c>
       <c r="AG150" t="s">
-        <v>207</v>
+        <v>773</v>
       </c>
       <c r="AH150" t="s">
-        <v>1027</v>
+        <v>370</v>
       </c>
       <c r="AI150" s="1">
-        <v>0.72916666666666663</v>
+        <v>0.625</v>
       </c>
       <c r="AJ150">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AL150" t="s">
         <v>1029</v>
       </c>
       <c r="AN150" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="AO150" t="s">
-        <v>1030</v>
+        <v>1037</v>
       </c>
       <c r="AQ150">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="AR150" s="1">
-        <v>5.2083333333333336E-2</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="AS150" s="1">
-        <v>0.875</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="AT150" t="s">
-        <v>1031</v>
+        <v>58</v>
       </c>
     </row>
     <row r="151" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
-        <v>1032</v>
+        <v>1038</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>1032</v>
+        <v>1038</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>1033</v>
+        <v>1038</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>1034</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>1032</v>
+        <v>1038</v>
       </c>
       <c r="F151" s="3" t="s">
         <v>1032</v>
@@ -22529,11 +22529,11 @@
       <c r="I151" t="s">
         <v>1036</v>
       </c>
-      <c r="J151" s="6" t="s">
-        <v>1119</v>
+      <c r="J151" s="3" t="s">
+        <v>1121</v>
       </c>
       <c r="K151" s="5">
-        <v>0.85</v>
+        <v>0.25</v>
       </c>
       <c r="L151" s="5" t="s">
         <v>45</v>
@@ -22542,13 +22542,13 @@
         <v>0</v>
       </c>
       <c r="N151" s="5">
-        <v>1.47</v>
+        <v>0.2</v>
       </c>
       <c r="O151" s="5" t="s">
         <v>45</v>
       </c>
       <c r="P151" s="5">
-        <v>0.04</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="Q151" s="5" t="s">
         <v>45</v>
@@ -22557,7 +22557,7 @@
         <v>46</v>
       </c>
       <c r="S151">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="T151" t="s">
         <v>78</v>
@@ -22575,7 +22575,7 @@
         <v>1</v>
       </c>
       <c r="Z151">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="AA151" t="s">
         <v>49</v>
@@ -22614,10 +22614,10 @@
         <v>56</v>
       </c>
       <c r="AO151" t="s">
-        <v>1037</v>
+        <v>1039</v>
       </c>
       <c r="AQ151">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="AR151" s="1">
         <v>0.29166666666666669</v>
@@ -22631,67 +22631,59 @@
     </row>
     <row r="152" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>1038</v>
+        <v>1041</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>1034</v>
+        <v>315</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>1032</v>
+        <v>1042</v>
       </c>
       <c r="H152" t="s">
-        <v>45</v>
+        <v>258</v>
       </c>
       <c r="I152" t="s">
-        <v>1036</v>
+        <v>1043</v>
       </c>
       <c r="J152" s="3" t="s">
-        <v>1121</v>
+        <v>1116</v>
       </c>
       <c r="K152" s="5">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="L152" s="5" t="s">
-        <v>45</v>
+        <v>258</v>
       </c>
       <c r="M152" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="N152" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="O152" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="P152" s="5">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="Q152" s="5" t="s">
-        <v>45</v>
-      </c>
+      <c r="N152" s="5"/>
+      <c r="O152" s="5"/>
+      <c r="P152" s="5"/>
+      <c r="Q152" s="5"/>
       <c r="R152" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="S152">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="T152" t="s">
-        <v>78</v>
+        <v>729</v>
       </c>
       <c r="U152" t="s">
-        <v>78</v>
+        <v>760</v>
       </c>
       <c r="V152" t="s">
-        <v>1035</v>
+        <v>731</v>
       </c>
       <c r="X152" t="b">
         <v>1</v>
@@ -22700,124 +22692,132 @@
         <v>1</v>
       </c>
       <c r="Z152">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="AA152" t="s">
-        <v>49</v>
+        <v>272</v>
       </c>
       <c r="AB152" t="s">
-        <v>49</v>
+        <v>272</v>
       </c>
       <c r="AC152">
-        <v>-60</v>
+        <v>-5</v>
       </c>
       <c r="AD152">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AE152">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AF152" t="s">
+        <v>703</v>
+      </c>
+      <c r="AG152" t="s">
+        <v>619</v>
+      </c>
+      <c r="AH152" t="s">
+        <v>704</v>
+      </c>
+      <c r="AI152" s="1">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="AJ152">
+        <v>21</v>
+      </c>
+      <c r="AL152" t="s">
+        <v>506</v>
+      </c>
+      <c r="AM152" t="s">
+        <v>724</v>
+      </c>
+      <c r="AN152" t="s">
+        <v>72</v>
+      </c>
+      <c r="AO152" t="s">
+        <v>1044</v>
+      </c>
+      <c r="AQ152">
         <v>50</v>
       </c>
-      <c r="AG152" t="s">
-        <v>773</v>
-      </c>
-      <c r="AH152" t="s">
-        <v>370</v>
-      </c>
-      <c r="AI152" s="1">
-        <v>0.625</v>
-      </c>
-      <c r="AJ152">
-        <v>22</v>
-      </c>
-      <c r="AL152" t="s">
-        <v>1029</v>
-      </c>
-      <c r="AN152" t="s">
-        <v>56</v>
-      </c>
-      <c r="AO152" t="s">
-        <v>1039</v>
-      </c>
-      <c r="AQ152">
-        <v>100</v>
-      </c>
       <c r="AR152" s="1">
-        <v>0.29166666666666669</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AS152" s="1">
-        <v>0.91666666666666663</v>
+        <v>0.87847222222222221</v>
       </c>
       <c r="AT152" t="s">
-        <v>58</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="153" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
-        <v>1040</v>
+        <v>995</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>1040</v>
+        <v>995</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>1041</v>
+        <v>995</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>315</v>
+        <v>89</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>1040</v>
-      </c>
-      <c r="F153" s="3" t="s">
-        <v>1042</v>
+        <v>995</v>
       </c>
       <c r="H153" t="s">
-        <v>258</v>
+        <v>45</v>
       </c>
       <c r="I153" t="s">
-        <v>1043</v>
-      </c>
-      <c r="J153" s="3" t="s">
-        <v>1116</v>
+        <v>997</v>
+      </c>
+      <c r="J153" s="6" t="s">
+        <v>1119</v>
       </c>
       <c r="K153" s="5">
-        <v>2</v>
+        <v>0.85</v>
       </c>
       <c r="L153" s="5" t="s">
-        <v>258</v>
+        <v>45</v>
       </c>
       <c r="M153" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="N153" s="5"/>
-      <c r="O153" s="5"/>
-      <c r="P153" s="5"/>
-      <c r="Q153" s="5"/>
+      <c r="N153" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="O153" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="P153" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="Q153" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="R153" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="S153">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="T153" t="s">
-        <v>729</v>
+        <v>996</v>
       </c>
       <c r="U153" t="s">
-        <v>760</v>
+        <v>996</v>
       </c>
       <c r="V153" t="s">
-        <v>731</v>
+        <v>996</v>
       </c>
       <c r="X153" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y153">
         <v>1</v>
       </c>
       <c r="Z153">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="AA153" t="s">
         <v>272</v>
@@ -22826,52 +22826,49 @@
         <v>272</v>
       </c>
       <c r="AC153">
-        <v>-5</v>
+        <v>-18</v>
       </c>
       <c r="AD153">
-        <v>16</v>
+        <v>1844</v>
       </c>
       <c r="AE153">
         <v>1</v>
       </c>
       <c r="AF153" t="s">
-        <v>703</v>
+        <v>50</v>
       </c>
       <c r="AG153" t="s">
-        <v>619</v>
+        <v>51</v>
       </c>
       <c r="AH153" t="s">
-        <v>704</v>
+        <v>370</v>
       </c>
       <c r="AI153" s="1">
-        <v>0.72916666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="AJ153">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AL153" t="s">
-        <v>506</v>
+        <v>998</v>
       </c>
       <c r="AM153" t="s">
-        <v>724</v>
+        <v>277</v>
       </c>
       <c r="AN153" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="AO153" t="s">
-        <v>1044</v>
+        <v>999</v>
       </c>
       <c r="AQ153">
-        <v>50</v>
+        <v>1000</v>
       </c>
       <c r="AR153" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="AS153" s="1">
-        <v>0.87847222222222221</v>
-      </c>
-      <c r="AT153" t="s">
-        <v>1045</v>
+        <v>0.91666666666666663</v>
       </c>
     </row>
     <row r="154" spans="1:46" x14ac:dyDescent="0.2">

</xml_diff>